<commit_message>
Adds minichart logic to xlsx writer
</commit_message>
<xml_diff>
--- a/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample16-1.xlsx
+++ b/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample16-1.xlsx
@@ -939,5 +939,27 @@
   <pageMargins left="20" right="20" top="20" bottom="20" header="0.315" footer="0.315"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
+  <extLst>
+    <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
+      <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{297a0399-daad-416e-b172-fe47b23eb5c3}" type="line" high="1" displayXAxis="1">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF0000FF"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFFF0000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'SEKRates'!B2:B12</xm:f>
+              <xm:sqref>B14</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+      </x14:sparklineGroups>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
xlsx writer updated for support minicharts (in progress..)
</commit_message>
<xml_diff>
--- a/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample16-1.xlsx
+++ b/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample16-1.xlsx
@@ -942,10 +942,10 @@
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{297a0399-daad-416e-b172-fe47b23eb5c3}" type="line" high="1" displayXAxis="1">
-          <x14:colorSeries rgb="FF376092"/>
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2519cc17-ce64-4fd1-aacc-ebe8035a82e7}" type="line" displayHidden="0" displayEmptyCellsAs="gap" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+          <x14:colorSeries rgb="0"/>
           <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF0000FF"/>
+          <x14:colorAxis rgb="FF000000"/>
           <x14:colorMarkers rgb="FFD00000"/>
           <x14:colorFirst rgb="FFD00000"/>
           <x14:colorLast rgb="FFD00000"/>
@@ -957,6 +957,7 @@
               <xm:sqref>B14</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
+          <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>

</xml_diff>

<commit_message>
Mini-Chart development finished (in test), Adds Maximum and Minimum Criterias in xsd and code (in test)
</commit_message>
<xml_diff>
--- a/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample16-1.xlsx
+++ b/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample16-1.xlsx
@@ -101,7 +101,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,6 +123,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00" tint="0"/>
+        <bgColor rgb="FFFFFF" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000" tint="0"/>
+        <bgColor rgb="FFFFFF" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000" tint="0"/>
         <bgColor rgb="FFFFFF" tint="0"/>
       </patternFill>
     </fill>
@@ -167,7 +179,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2">
       <alignment horizontal="left" vertical="center"/>
@@ -208,8 +220,14 @@
     <xf numFmtId="165" fontId="3" fillId="4" borderId="2">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="3" fillId="5" borderId="2">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="6" borderId="2">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0"/>
     <xf numFmtId="49" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" xfId="1">
       <alignment horizontal="left" vertical="center"/>
@@ -250,8 +268,14 @@
     <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="2" applyBorder="1" xfId="13">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="5" applyFill="1" borderId="2" applyBorder="1" xfId="14">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="6" applyFill="1" borderId="2" applyBorder="1" xfId="15">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="16">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="_Default_" xfId="1"/>
     <cellStyle name="HeaderStyle" xfId="2"/>
@@ -266,6 +290,8 @@
     <cellStyle name="LastFiedlDecimalValueStyle_Alternate" xfId="11"/>
     <cellStyle name="RemarksMYRStyle" xfId="12"/>
     <cellStyle name="RemarksMYRStyle_Alternate" xfId="13"/>
+    <cellStyle name="MaximumMYRStyle" xfId="14"/>
+    <cellStyle name="MaximumMYRStyle_Alternate" xfId="15"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
@@ -352,585 +378,585 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4">
+      <c r="A2" s="0">
         <v>42430</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="0">
         <v>6.1735000610351562</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="0">
         <v>6.420839786529541</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="0">
         <v>8.6478500366210937</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="0">
         <v>1.2566800117492676</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="0">
         <v>9.3737602233886719</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="0">
         <v>12.016830444335938</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="0">
         <v>1.1106699705123901</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="0">
         <v>0.075989998877048492</v>
       </c>
       <c r="J2" s="6">
         <v>2.0690000057220459</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="0">
         <v>0.99522000551223755</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="0">
         <v>5.6922698020935059</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="0">
         <v>0.11665000021457672</v>
       </c>
-      <c r="N2" s="8">
-        <v>1</v>
-      </c>
-      <c r="O2" s="6">
+      <c r="N2" s="0">
+        <v>1</v>
+      </c>
+      <c r="O2" s="0">
         <v>0.24232999980449677</v>
       </c>
-      <c r="P2" s="6">
+      <c r="P2" s="0">
         <v>2.9301700592041016</v>
       </c>
-      <c r="Q2" s="10">
+      <c r="Q2" s="0">
         <v>8.6318502426147461</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5">
+      <c r="A3" s="0">
         <v>42431</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="0">
         <v>6.27223014831543</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="0">
         <v>6.4234499931335449</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="0">
         <v>8.63479995727539</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="0">
         <v>1.254040002822876</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="0">
         <v>9.3535003662109375</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="0">
         <v>12.149700164794922</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="0">
         <v>1.110990047454834</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="0">
         <v>0.075819998979568481</v>
       </c>
       <c r="J3" s="7">
         <v>2.074009895324707</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="0">
         <v>0.99311000108718872</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="0">
         <v>5.7327699661254883</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="0">
         <v>0.11756999790668488</v>
       </c>
-      <c r="N3" s="9">
-        <v>1</v>
-      </c>
-      <c r="O3" s="7">
+      <c r="N3" s="0">
+        <v>1</v>
+      </c>
+      <c r="O3" s="0">
         <v>0.24305999279022217</v>
       </c>
-      <c r="P3" s="7">
+      <c r="P3" s="0">
         <v>2.9408299922943115</v>
       </c>
-      <c r="Q3" s="11">
+      <c r="Q3" s="0">
         <v>8.6381998062133789</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4">
+      <c r="A4" s="0">
         <v>42436</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="0">
         <v>6.3377799987792969</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="0">
         <v>6.3840298652648926</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="0">
         <v>8.5024499893188477</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="0">
         <v>1.2497999668121338</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="0">
         <v>9.32373046875</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="0">
         <v>12.057559967041016</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="0">
         <v>1.0931400060653687</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="0">
         <v>0.074780002236366272</v>
       </c>
       <c r="J4" s="6">
         <v>2.0717101097106934</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="0">
         <v>0.99751001596450806</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="0">
         <v>5.7753901481628418</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="0">
         <v>0.11841999739408493</v>
       </c>
-      <c r="N4" s="8">
-        <v>1</v>
-      </c>
-      <c r="O4" s="6">
+      <c r="N4" s="0">
+        <v>1</v>
+      </c>
+      <c r="O4" s="0">
         <v>0.23973000049591064</v>
       </c>
-      <c r="P4" s="6">
+      <c r="P4" s="0">
         <v>2.9108800888061523</v>
       </c>
-      <c r="Q4" s="10">
+      <c r="Q4" s="0">
         <v>8.4888496398925781</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5">
+      <c r="A5" s="0">
         <v>42437</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="0">
         <v>6.3026800155639648</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="0">
         <v>6.3177399635314941</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="0">
         <v>8.54065990447998</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="0">
         <v>1.2547099590301514</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="0">
         <v>9.3625402450561523</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="0">
         <v>12.033610343933105</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="0">
         <v>1.090459942817688</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="0">
         <v>0.075309999287128448</v>
       </c>
       <c r="J5" s="7">
         <v>2.0562500953674316</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="0">
         <v>0.99225002527236938</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="0">
         <v>5.7250099182128906</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="0">
         <v>0.11619000136852264</v>
       </c>
-      <c r="N5" s="9">
-        <v>1</v>
-      </c>
-      <c r="O5" s="7">
+      <c r="N5" s="0">
+        <v>1</v>
+      </c>
+      <c r="O5" s="0">
         <v>0.23948000371456146</v>
       </c>
-      <c r="P5" s="7">
+      <c r="P5" s="0">
         <v>2.9106700420379639</v>
       </c>
-      <c r="Q5" s="11">
+      <c r="Q5" s="0">
         <v>8.4701995849609375</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4">
+      <c r="A6" s="0">
         <v>42438</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="0">
         <v>6.3263001441955566</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="0">
         <v>6.336979866027832</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="0">
         <v>8.4611797332763672</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="0">
         <v>1.2439899444580078</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="0">
         <v>9.28125</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="0">
         <v>11.988789558410645</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="0">
         <v>1.0854400396347046</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="0">
         <v>0.074670001864433289</v>
       </c>
       <c r="J6" s="6">
         <v>2.0412800312042236</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="0">
         <v>0.98960000276565552</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="0">
         <v>5.7160100936889648</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="0">
         <v>0.11862999945878983</v>
       </c>
-      <c r="N6" s="8">
-        <v>1</v>
-      </c>
-      <c r="O6" s="6">
+      <c r="N6" s="0">
+        <v>1</v>
+      </c>
+      <c r="O6" s="0">
         <v>0.23893000185489655</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P6" s="0">
         <v>2.9134900569915771</v>
       </c>
-      <c r="Q6" s="10">
+      <c r="Q6" s="0">
         <v>8.4294500350952148</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5">
+      <c r="A7" s="0">
         <v>42439</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="0">
         <v>6.2424101829528809</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="0">
         <v>6.2881698608398437</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="0">
         <v>8.48684024810791</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="0">
         <v>1.2525999546051025</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="0">
         <v>9.3435001373291016</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="0">
         <v>11.99193000793457</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="0">
         <v>1.0795600414276123</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="0">
         <v>0.073919996619224548</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="7">
         <v>2.0450000762939453</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="0">
         <v>0.9826700091362</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="0">
         <v>5.58144998550415</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="0">
         <v>0.11768999695777893</v>
       </c>
-      <c r="N7" s="9">
-        <v>1</v>
-      </c>
-      <c r="O7" s="7">
+      <c r="N7" s="0">
+        <v>1</v>
+      </c>
+      <c r="O7" s="0">
         <v>0.2378000020980835</v>
       </c>
-      <c r="P7" s="7">
+      <c r="P7" s="0">
         <v>2.8914999961853027</v>
       </c>
-      <c r="Q7" s="11">
+      <c r="Q7" s="0">
         <v>8.3824501037597656</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4">
+      <c r="A8" s="0">
         <v>42440</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="0">
         <v>6.3017997741699219</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="0">
         <v>6.3015198707580566</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="0">
         <v>8.4829502105712891</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="0">
         <v>1.248479962348938</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="0">
         <v>9.3122997283935547</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="0">
         <v>12.011940002441406</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="0">
         <v>1.0754499435424805</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="0">
         <v>0.0735199972987175</v>
       </c>
       <c r="J8" s="6">
         <v>2.0411200523376465</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="0">
         <v>0.98934000730514526</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="0">
         <v>5.6233501434326172</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="0">
         <v>0.11913999915122986</v>
       </c>
-      <c r="N8" s="8">
-        <v>1</v>
-      </c>
-      <c r="O8" s="6">
+      <c r="N8" s="0">
+        <v>1</v>
+      </c>
+      <c r="O8" s="0">
         <v>0.23808999359607697</v>
       </c>
-      <c r="P8" s="6">
+      <c r="P8" s="0">
         <v>2.90310001373291</v>
       </c>
-      <c r="Q8" s="10">
+      <c r="Q8" s="0">
         <v>8.3451004028320312</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="5">
+      <c r="A9" s="0">
         <v>42444</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="0">
         <v>6.19789981842041</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="0">
         <v>6.2161498069763184</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="0">
         <v>8.4293098449707031</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="0">
         <v>1.2375400066375732</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="0">
         <v>9.2289600372314453</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="0">
         <v>11.764180183410645</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="0">
         <v>1.0702600479125977</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="0">
         <v>0.0735900029540062</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="14">
         <v>2.0092899799346924</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="0">
         <v>0.9712899923324585</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9" s="0">
         <v>5.4927802085876465</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="0">
         <v>0.11693999916315079</v>
       </c>
-      <c r="N9" s="9">
-        <v>1</v>
-      </c>
-      <c r="O9" s="7">
+      <c r="N9" s="0">
+        <v>1</v>
+      </c>
+      <c r="O9" s="0">
         <v>0.23642000555992126</v>
       </c>
-      <c r="P9" s="7">
+      <c r="P9" s="0">
         <v>2.8648700714111328</v>
       </c>
-      <c r="Q9" s="11">
+      <c r="Q9" s="0">
         <v>8.3053998947143555</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4">
+      <c r="A10" s="0">
         <v>42445</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="0">
         <v>6.1850800514221191</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="0">
         <v>6.2249298095703125</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="0">
         <v>8.4179201126098633</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="0">
         <v>1.2354300022125244</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="0">
         <v>9.2114896774292</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="0">
         <v>11.724699974060059</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="0">
         <v>1.0715199708938599</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="0">
         <v>0.073179997503757477</v>
       </c>
       <c r="J10" s="6">
         <v>2.0117900371551514</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="0">
         <v>0.96907001733779907</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="0">
         <v>5.4913802146911621</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="0">
         <v>0.1183599978685379</v>
       </c>
-      <c r="N10" s="8">
-        <v>1</v>
-      </c>
-      <c r="O10" s="6">
+      <c r="N10" s="0">
+        <v>1</v>
+      </c>
+      <c r="O10" s="0">
         <v>0.23724000155925751</v>
       </c>
-      <c r="P10" s="6">
+      <c r="P10" s="0">
         <v>2.8476700782775879</v>
       </c>
-      <c r="Q10" s="10">
+      <c r="Q10" s="0">
         <v>8.3177499771118164</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="5">
+      <c r="A11" s="0">
         <v>42446</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="0">
         <v>6.2521400451660156</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="0">
         <v>6.306419849395752</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="0">
         <v>8.4598102569580078</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="0">
         <v>1.2432700395584106</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="0">
         <v>9.2662296295166016</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="0">
         <v>11.863960266113281</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="0">
         <v>1.0557099580764771</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="0">
         <v>0.073559999465942383</v>
       </c>
       <c r="J11" s="7">
         <v>2.0170600414276123</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="0">
         <v>0.98158997297286987</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="0">
         <v>5.5954399108886719</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="0">
         <v>0.12024000287055969</v>
       </c>
-      <c r="N11" s="9">
-        <v>1</v>
-      </c>
-      <c r="O11" s="7">
+      <c r="N11" s="0">
+        <v>1</v>
+      </c>
+      <c r="O11" s="0">
         <v>0.23543000221252441</v>
       </c>
-      <c r="P11" s="7">
+      <c r="P11" s="0">
         <v>2.8759500980377197</v>
       </c>
-      <c r="Q11" s="11">
+      <c r="Q11" s="0">
         <v>8.1882495880126953</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4">
+      <c r="A12" s="0">
         <v>42447</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="0">
         <v>6.2535901069641113</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="0">
         <v>6.3239998817443848</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="0">
         <v>8.4782600402832031</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="0">
         <v>1.2438100576400757</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="0">
         <v>9.2697601318359375</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="0">
         <v>11.913220405578613</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="0">
         <v>1.0588099956512451</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="0">
         <v>0.073700003325939178</v>
       </c>
       <c r="J12" s="6">
         <v>2.0255401134490967</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="0">
         <v>0.9843900203704834</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="0">
         <v>5.590670108795166</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M12" s="0">
         <v>0.12063000351190567</v>
       </c>
-      <c r="N12" s="8">
-        <v>1</v>
-      </c>
-      <c r="O12" s="6">
+      <c r="N12" s="0">
+        <v>1</v>
+      </c>
+      <c r="O12" s="0">
         <v>0.23537999391555786</v>
       </c>
-      <c r="P12" s="6">
+      <c r="P12" s="0">
         <v>2.8687999248504639</v>
       </c>
-      <c r="Q12" s="10">
+      <c r="Q12" s="0">
         <v>8.2095003128051758</v>
       </c>
     </row>
@@ -942,7 +968,7 @@
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2519cc17-ce64-4fd1-aacc-ebe8035a82e7}" type="line" displayHidden="0" displayEmptyCellsAs="gap" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4f2b2c4b-a20f-4e69-948e-94f85c370af0}" type="line" displayHidden="0" displayEmptyCellsAs="zero" rightToLeft="0" displayXAxis="1" dateAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="0"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -951,6 +977,7 @@
           <x14:colorLast rgb="FFD00000"/>
           <x14:colorHigh rgb="FFFF0000"/>
           <x14:colorLow rgb="FFD00000"/>
+          <xm:f>'SEKRates'!A2:A12</xm:f>
           <x14:sparklines>
             <x14:sparkline>
               <xm:f>'SEKRates'!B2:B12</xm:f>

</xml_diff>

<commit_message>
Reorder all model classes into Model folder, minor changes in min/max/zero conditions
</commit_message>
<xml_diff>
--- a/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample16-1.xlsx
+++ b/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample16-1.xlsx
@@ -378,585 +378,585 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0">
+      <c r="A2" s="4">
         <v>42430</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2" s="6">
         <v>6.1735000610351562</v>
       </c>
-      <c r="C2" s="0">
+      <c r="C2" s="6">
         <v>6.420839786529541</v>
       </c>
-      <c r="D2" s="0">
+      <c r="D2" s="6">
         <v>8.6478500366210937</v>
       </c>
-      <c r="E2" s="0">
+      <c r="E2" s="6">
         <v>1.2566800117492676</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F2" s="6">
         <v>9.3737602233886719</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G2" s="6">
         <v>12.016830444335938</v>
       </c>
-      <c r="H2" s="0">
+      <c r="H2" s="6">
         <v>1.1106699705123901</v>
       </c>
-      <c r="I2" s="0">
+      <c r="I2" s="6">
         <v>0.075989998877048492</v>
       </c>
       <c r="J2" s="6">
         <v>2.0690000057220459</v>
       </c>
-      <c r="K2" s="0">
+      <c r="K2" s="6">
         <v>0.99522000551223755</v>
       </c>
-      <c r="L2" s="0">
+      <c r="L2" s="6">
         <v>5.6922698020935059</v>
       </c>
-      <c r="M2" s="0">
+      <c r="M2" s="6">
         <v>0.11665000021457672</v>
       </c>
-      <c r="N2" s="0">
-        <v>1</v>
-      </c>
-      <c r="O2" s="0">
+      <c r="N2" s="8">
+        <v>1</v>
+      </c>
+      <c r="O2" s="6">
         <v>0.24232999980449677</v>
       </c>
-      <c r="P2" s="0">
+      <c r="P2" s="6">
         <v>2.9301700592041016</v>
       </c>
-      <c r="Q2" s="0">
+      <c r="Q2" s="10">
         <v>8.6318502426147461</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0">
+      <c r="A3" s="5">
         <v>42431</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3" s="7">
         <v>6.27223014831543</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3" s="7">
         <v>6.4234499931335449</v>
       </c>
-      <c r="D3" s="0">
+      <c r="D3" s="7">
         <v>8.63479995727539</v>
       </c>
-      <c r="E3" s="0">
+      <c r="E3" s="7">
         <v>1.254040002822876</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3" s="7">
         <v>9.3535003662109375</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G3" s="7">
         <v>12.149700164794922</v>
       </c>
-      <c r="H3" s="0">
+      <c r="H3" s="7">
         <v>1.110990047454834</v>
       </c>
-      <c r="I3" s="0">
+      <c r="I3" s="7">
         <v>0.075819998979568481</v>
       </c>
       <c r="J3" s="14">
         <v>2.074009895324707</v>
       </c>
-      <c r="K3" s="0">
+      <c r="K3" s="7">
         <v>0.99311000108718872</v>
       </c>
-      <c r="L3" s="0">
+      <c r="L3" s="7">
         <v>5.7327699661254883</v>
       </c>
-      <c r="M3" s="0">
+      <c r="M3" s="7">
         <v>0.11756999790668488</v>
       </c>
-      <c r="N3" s="0">
-        <v>1</v>
-      </c>
-      <c r="O3" s="0">
+      <c r="N3" s="9">
+        <v>1</v>
+      </c>
+      <c r="O3" s="7">
         <v>0.24305999279022217</v>
       </c>
-      <c r="P3" s="0">
+      <c r="P3" s="7">
         <v>2.9408299922943115</v>
       </c>
-      <c r="Q3" s="0">
+      <c r="Q3" s="11">
         <v>8.6381998062133789</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0">
+      <c r="A4" s="4">
         <v>42436</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4" s="6">
         <v>6.3377799987792969</v>
       </c>
-      <c r="C4" s="0">
+      <c r="C4" s="6">
         <v>6.3840298652648926</v>
       </c>
-      <c r="D4" s="0">
+      <c r="D4" s="6">
         <v>8.5024499893188477</v>
       </c>
-      <c r="E4" s="0">
+      <c r="E4" s="6">
         <v>1.2497999668121338</v>
       </c>
-      <c r="F4" s="0">
+      <c r="F4" s="6">
         <v>9.32373046875</v>
       </c>
-      <c r="G4" s="0">
+      <c r="G4" s="6">
         <v>12.057559967041016</v>
       </c>
-      <c r="H4" s="0">
+      <c r="H4" s="6">
         <v>1.0931400060653687</v>
       </c>
-      <c r="I4" s="0">
+      <c r="I4" s="6">
         <v>0.074780002236366272</v>
       </c>
       <c r="J4" s="6">
         <v>2.0717101097106934</v>
       </c>
-      <c r="K4" s="0">
+      <c r="K4" s="6">
         <v>0.99751001596450806</v>
       </c>
-      <c r="L4" s="0">
+      <c r="L4" s="6">
         <v>5.7753901481628418</v>
       </c>
-      <c r="M4" s="0">
+      <c r="M4" s="6">
         <v>0.11841999739408493</v>
       </c>
-      <c r="N4" s="0">
-        <v>1</v>
-      </c>
-      <c r="O4" s="0">
+      <c r="N4" s="8">
+        <v>1</v>
+      </c>
+      <c r="O4" s="6">
         <v>0.23973000049591064</v>
       </c>
-      <c r="P4" s="0">
+      <c r="P4" s="6">
         <v>2.9108800888061523</v>
       </c>
-      <c r="Q4" s="0">
+      <c r="Q4" s="10">
         <v>8.4888496398925781</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0">
+      <c r="A5" s="5">
         <v>42437</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5" s="7">
         <v>6.3026800155639648</v>
       </c>
-      <c r="C5" s="0">
+      <c r="C5" s="7">
         <v>6.3177399635314941</v>
       </c>
-      <c r="D5" s="0">
+      <c r="D5" s="7">
         <v>8.54065990447998</v>
       </c>
-      <c r="E5" s="0">
+      <c r="E5" s="7">
         <v>1.2547099590301514</v>
       </c>
-      <c r="F5" s="0">
+      <c r="F5" s="7">
         <v>9.3625402450561523</v>
       </c>
-      <c r="G5" s="0">
+      <c r="G5" s="7">
         <v>12.033610343933105</v>
       </c>
-      <c r="H5" s="0">
+      <c r="H5" s="7">
         <v>1.090459942817688</v>
       </c>
-      <c r="I5" s="0">
+      <c r="I5" s="7">
         <v>0.075309999287128448</v>
       </c>
       <c r="J5" s="7">
         <v>2.0562500953674316</v>
       </c>
-      <c r="K5" s="0">
+      <c r="K5" s="7">
         <v>0.99225002527236938</v>
       </c>
-      <c r="L5" s="0">
+      <c r="L5" s="7">
         <v>5.7250099182128906</v>
       </c>
-      <c r="M5" s="0">
+      <c r="M5" s="7">
         <v>0.11619000136852264</v>
       </c>
-      <c r="N5" s="0">
-        <v>1</v>
-      </c>
-      <c r="O5" s="0">
+      <c r="N5" s="9">
+        <v>1</v>
+      </c>
+      <c r="O5" s="7">
         <v>0.23948000371456146</v>
       </c>
-      <c r="P5" s="0">
+      <c r="P5" s="7">
         <v>2.9106700420379639</v>
       </c>
-      <c r="Q5" s="0">
+      <c r="Q5" s="11">
         <v>8.4701995849609375</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0">
+      <c r="A6" s="4">
         <v>42438</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6" s="6">
         <v>6.3263001441955566</v>
       </c>
-      <c r="C6" s="0">
+      <c r="C6" s="6">
         <v>6.336979866027832</v>
       </c>
-      <c r="D6" s="0">
+      <c r="D6" s="6">
         <v>8.4611797332763672</v>
       </c>
-      <c r="E6" s="0">
+      <c r="E6" s="6">
         <v>1.2439899444580078</v>
       </c>
-      <c r="F6" s="0">
+      <c r="F6" s="6">
         <v>9.28125</v>
       </c>
-      <c r="G6" s="0">
+      <c r="G6" s="6">
         <v>11.988789558410645</v>
       </c>
-      <c r="H6" s="0">
+      <c r="H6" s="6">
         <v>1.0854400396347046</v>
       </c>
-      <c r="I6" s="0">
+      <c r="I6" s="6">
         <v>0.074670001864433289</v>
       </c>
       <c r="J6" s="6">
         <v>2.0412800312042236</v>
       </c>
-      <c r="K6" s="0">
+      <c r="K6" s="6">
         <v>0.98960000276565552</v>
       </c>
-      <c r="L6" s="0">
+      <c r="L6" s="6">
         <v>5.7160100936889648</v>
       </c>
-      <c r="M6" s="0">
+      <c r="M6" s="6">
         <v>0.11862999945878983</v>
       </c>
-      <c r="N6" s="0">
-        <v>1</v>
-      </c>
-      <c r="O6" s="0">
+      <c r="N6" s="8">
+        <v>1</v>
+      </c>
+      <c r="O6" s="6">
         <v>0.23893000185489655</v>
       </c>
-      <c r="P6" s="0">
+      <c r="P6" s="6">
         <v>2.9134900569915771</v>
       </c>
-      <c r="Q6" s="0">
+      <c r="Q6" s="10">
         <v>8.4294500350952148</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="0">
+      <c r="A7" s="5">
         <v>42439</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7" s="7">
         <v>6.2424101829528809</v>
       </c>
-      <c r="C7" s="0">
+      <c r="C7" s="7">
         <v>6.2881698608398437</v>
       </c>
-      <c r="D7" s="0">
+      <c r="D7" s="7">
         <v>8.48684024810791</v>
       </c>
-      <c r="E7" s="0">
+      <c r="E7" s="7">
         <v>1.2525999546051025</v>
       </c>
-      <c r="F7" s="0">
+      <c r="F7" s="7">
         <v>9.3435001373291016</v>
       </c>
-      <c r="G7" s="0">
+      <c r="G7" s="7">
         <v>11.99193000793457</v>
       </c>
-      <c r="H7" s="0">
+      <c r="H7" s="7">
         <v>1.0795600414276123</v>
       </c>
-      <c r="I7" s="0">
+      <c r="I7" s="7">
         <v>0.073919996619224548</v>
       </c>
       <c r="J7" s="7">
         <v>2.0450000762939453</v>
       </c>
-      <c r="K7" s="0">
+      <c r="K7" s="7">
         <v>0.9826700091362</v>
       </c>
-      <c r="L7" s="0">
+      <c r="L7" s="7">
         <v>5.58144998550415</v>
       </c>
-      <c r="M7" s="0">
+      <c r="M7" s="7">
         <v>0.11768999695777893</v>
       </c>
-      <c r="N7" s="0">
-        <v>1</v>
-      </c>
-      <c r="O7" s="0">
+      <c r="N7" s="9">
+        <v>1</v>
+      </c>
+      <c r="O7" s="7">
         <v>0.2378000020980835</v>
       </c>
-      <c r="P7" s="0">
+      <c r="P7" s="7">
         <v>2.8914999961853027</v>
       </c>
-      <c r="Q7" s="0">
+      <c r="Q7" s="11">
         <v>8.3824501037597656</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="0">
+      <c r="A8" s="4">
         <v>42440</v>
       </c>
-      <c r="B8" s="0">
+      <c r="B8" s="6">
         <v>6.3017997741699219</v>
       </c>
-      <c r="C8" s="0">
+      <c r="C8" s="6">
         <v>6.3015198707580566</v>
       </c>
-      <c r="D8" s="0">
+      <c r="D8" s="6">
         <v>8.4829502105712891</v>
       </c>
-      <c r="E8" s="0">
+      <c r="E8" s="6">
         <v>1.248479962348938</v>
       </c>
-      <c r="F8" s="0">
+      <c r="F8" s="6">
         <v>9.3122997283935547</v>
       </c>
-      <c r="G8" s="0">
+      <c r="G8" s="6">
         <v>12.011940002441406</v>
       </c>
-      <c r="H8" s="0">
+      <c r="H8" s="6">
         <v>1.0754499435424805</v>
       </c>
-      <c r="I8" s="0">
+      <c r="I8" s="6">
         <v>0.0735199972987175</v>
       </c>
       <c r="J8" s="6">
         <v>2.0411200523376465</v>
       </c>
-      <c r="K8" s="0">
+      <c r="K8" s="6">
         <v>0.98934000730514526</v>
       </c>
-      <c r="L8" s="0">
+      <c r="L8" s="6">
         <v>5.6233501434326172</v>
       </c>
-      <c r="M8" s="0">
+      <c r="M8" s="6">
         <v>0.11913999915122986</v>
       </c>
-      <c r="N8" s="0">
-        <v>1</v>
-      </c>
-      <c r="O8" s="0">
+      <c r="N8" s="8">
+        <v>1</v>
+      </c>
+      <c r="O8" s="6">
         <v>0.23808999359607697</v>
       </c>
-      <c r="P8" s="0">
+      <c r="P8" s="6">
         <v>2.90310001373291</v>
       </c>
-      <c r="Q8" s="0">
+      <c r="Q8" s="10">
         <v>8.3451004028320312</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="0">
+      <c r="A9" s="5">
         <v>42444</v>
       </c>
-      <c r="B9" s="0">
+      <c r="B9" s="7">
         <v>6.19789981842041</v>
       </c>
-      <c r="C9" s="0">
+      <c r="C9" s="7">
         <v>6.2161498069763184</v>
       </c>
-      <c r="D9" s="0">
+      <c r="D9" s="7">
         <v>8.4293098449707031</v>
       </c>
-      <c r="E9" s="0">
+      <c r="E9" s="7">
         <v>1.2375400066375732</v>
       </c>
-      <c r="F9" s="0">
+      <c r="F9" s="7">
         <v>9.2289600372314453</v>
       </c>
-      <c r="G9" s="0">
+      <c r="G9" s="7">
         <v>11.764180183410645</v>
       </c>
-      <c r="H9" s="0">
+      <c r="H9" s="7">
         <v>1.0702600479125977</v>
       </c>
-      <c r="I9" s="0">
+      <c r="I9" s="7">
         <v>0.0735900029540062</v>
       </c>
       <c r="J9" s="7">
         <v>2.0092899799346924</v>
       </c>
-      <c r="K9" s="0">
+      <c r="K9" s="7">
         <v>0.9712899923324585</v>
       </c>
-      <c r="L9" s="0">
+      <c r="L9" s="7">
         <v>5.4927802085876465</v>
       </c>
-      <c r="M9" s="0">
+      <c r="M9" s="7">
         <v>0.11693999916315079</v>
       </c>
-      <c r="N9" s="0">
-        <v>1</v>
-      </c>
-      <c r="O9" s="0">
+      <c r="N9" s="9">
+        <v>1</v>
+      </c>
+      <c r="O9" s="7">
         <v>0.23642000555992126</v>
       </c>
-      <c r="P9" s="0">
+      <c r="P9" s="7">
         <v>2.8648700714111328</v>
       </c>
-      <c r="Q9" s="0">
+      <c r="Q9" s="11">
         <v>8.3053998947143555</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="0">
+      <c r="A10" s="4">
         <v>42445</v>
       </c>
-      <c r="B10" s="0">
+      <c r="B10" s="6">
         <v>6.1850800514221191</v>
       </c>
-      <c r="C10" s="0">
+      <c r="C10" s="6">
         <v>6.2249298095703125</v>
       </c>
-      <c r="D10" s="0">
+      <c r="D10" s="6">
         <v>8.4179201126098633</v>
       </c>
-      <c r="E10" s="0">
+      <c r="E10" s="6">
         <v>1.2354300022125244</v>
       </c>
-      <c r="F10" s="0">
+      <c r="F10" s="6">
         <v>9.2114896774292</v>
       </c>
-      <c r="G10" s="0">
+      <c r="G10" s="6">
         <v>11.724699974060059</v>
       </c>
-      <c r="H10" s="0">
+      <c r="H10" s="6">
         <v>1.0715199708938599</v>
       </c>
-      <c r="I10" s="0">
+      <c r="I10" s="6">
         <v>0.073179997503757477</v>
       </c>
       <c r="J10" s="6">
         <v>2.0117900371551514</v>
       </c>
-      <c r="K10" s="0">
+      <c r="K10" s="6">
         <v>0.96907001733779907</v>
       </c>
-      <c r="L10" s="0">
+      <c r="L10" s="6">
         <v>5.4913802146911621</v>
       </c>
-      <c r="M10" s="0">
+      <c r="M10" s="6">
         <v>0.1183599978685379</v>
       </c>
-      <c r="N10" s="0">
-        <v>1</v>
-      </c>
-      <c r="O10" s="0">
+      <c r="N10" s="8">
+        <v>1</v>
+      </c>
+      <c r="O10" s="6">
         <v>0.23724000155925751</v>
       </c>
-      <c r="P10" s="0">
+      <c r="P10" s="6">
         <v>2.8476700782775879</v>
       </c>
-      <c r="Q10" s="0">
+      <c r="Q10" s="10">
         <v>8.3177499771118164</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="0">
+      <c r="A11" s="5">
         <v>42446</v>
       </c>
-      <c r="B11" s="0">
+      <c r="B11" s="7">
         <v>6.2521400451660156</v>
       </c>
-      <c r="C11" s="0">
+      <c r="C11" s="7">
         <v>6.306419849395752</v>
       </c>
-      <c r="D11" s="0">
+      <c r="D11" s="7">
         <v>8.4598102569580078</v>
       </c>
-      <c r="E11" s="0">
+      <c r="E11" s="7">
         <v>1.2432700395584106</v>
       </c>
-      <c r="F11" s="0">
+      <c r="F11" s="7">
         <v>9.2662296295166016</v>
       </c>
-      <c r="G11" s="0">
+      <c r="G11" s="7">
         <v>11.863960266113281</v>
       </c>
-      <c r="H11" s="0">
+      <c r="H11" s="7">
         <v>1.0557099580764771</v>
       </c>
-      <c r="I11" s="0">
+      <c r="I11" s="7">
         <v>0.073559999465942383</v>
       </c>
       <c r="J11" s="7">
         <v>2.0170600414276123</v>
       </c>
-      <c r="K11" s="0">
+      <c r="K11" s="7">
         <v>0.98158997297286987</v>
       </c>
-      <c r="L11" s="0">
+      <c r="L11" s="7">
         <v>5.5954399108886719</v>
       </c>
-      <c r="M11" s="0">
+      <c r="M11" s="7">
         <v>0.12024000287055969</v>
       </c>
-      <c r="N11" s="0">
-        <v>1</v>
-      </c>
-      <c r="O11" s="0">
+      <c r="N11" s="9">
+        <v>1</v>
+      </c>
+      <c r="O11" s="7">
         <v>0.23543000221252441</v>
       </c>
-      <c r="P11" s="0">
+      <c r="P11" s="7">
         <v>2.8759500980377197</v>
       </c>
-      <c r="Q11" s="0">
+      <c r="Q11" s="11">
         <v>8.1882495880126953</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="0">
+      <c r="A12" s="4">
         <v>42447</v>
       </c>
-      <c r="B12" s="0">
+      <c r="B12" s="6">
         <v>6.2535901069641113</v>
       </c>
-      <c r="C12" s="0">
+      <c r="C12" s="6">
         <v>6.3239998817443848</v>
       </c>
-      <c r="D12" s="0">
+      <c r="D12" s="6">
         <v>8.4782600402832031</v>
       </c>
-      <c r="E12" s="0">
+      <c r="E12" s="6">
         <v>1.2438100576400757</v>
       </c>
-      <c r="F12" s="0">
+      <c r="F12" s="6">
         <v>9.2697601318359375</v>
       </c>
-      <c r="G12" s="0">
+      <c r="G12" s="6">
         <v>11.913220405578613</v>
       </c>
-      <c r="H12" s="0">
+      <c r="H12" s="6">
         <v>1.0588099956512451</v>
       </c>
-      <c r="I12" s="0">
+      <c r="I12" s="6">
         <v>0.073700003325939178</v>
       </c>
       <c r="J12" s="6">
         <v>2.0255401134490967</v>
       </c>
-      <c r="K12" s="0">
+      <c r="K12" s="6">
         <v>0.9843900203704834</v>
       </c>
-      <c r="L12" s="0">
+      <c r="L12" s="6">
         <v>5.590670108795166</v>
       </c>
-      <c r="M12" s="0">
+      <c r="M12" s="6">
         <v>0.12063000351190567</v>
       </c>
-      <c r="N12" s="0">
-        <v>1</v>
-      </c>
-      <c r="O12" s="0">
+      <c r="N12" s="8">
+        <v>1</v>
+      </c>
+      <c r="O12" s="6">
         <v>0.23537999391555786</v>
       </c>
-      <c r="P12" s="0">
+      <c r="P12" s="6">
         <v>2.8687999248504639</v>
       </c>
-      <c r="Q12" s="0">
+      <c r="Q12" s="10">
         <v>8.2095003128051758</v>
       </c>
     </row>
@@ -968,7 +968,7 @@
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c61f2378-d621-479a-bc45-cc30556d2a5d}" type="line" displayHidden="0" displayEmptyCellsAs="zero" rightToLeft="0" displayXAxis="1" dateAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c962ee68-9a8e-41da-9f50-e83b3889586b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" rightToLeft="0" displayXAxis="1" dateAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="0"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>

<commit_message>
Adds Document metadata information into xsd and model classes, used in xslx writer, adds/modify header and footer document information in xsd and model classes. In progress...
</commit_message>
<xml_diff>
--- a/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample16-1.xlsx
+++ b/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample16-1.xlsx
@@ -9,7 +9,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SEKRates'!$A$1:$Q$1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'SEKRates'!$A$1:$Q$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'SEKRates'!$A$1:$Q$12</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'SEKRates'!$1:$1</definedName>
   </definedNames>
   <calcPr fullCalcOnLoad="1"/>
@@ -301,27 +301,27 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="1"/>
+    <sheetView workbookViewId="0" showGridLines="1" view="pageLayout"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.5485782623291" customWidth="1"/>
+    <col min="2" max="2" width="8.512770652771" customWidth="1"/>
+    <col min="3" max="3" width="8.512770652771" customWidth="1"/>
+    <col min="4" max="4" width="8.512770652771" customWidth="1"/>
+    <col min="5" max="5" width="8.512770652771" customWidth="1"/>
+    <col min="6" max="6" width="8.512770652771" customWidth="1"/>
     <col min="7" max="7" width="9.6064281463623" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="8.512770652771" customWidth="1"/>
+    <col min="9" max="9" width="8.512770652771" customWidth="1"/>
+    <col min="10" max="10" width="8.5311861038208" customWidth="1"/>
+    <col min="11" max="11" width="8.512770652771" customWidth="1"/>
+    <col min="12" max="12" width="8.512770652771" customWidth="1"/>
+    <col min="13" max="13" width="8.512770652771" customWidth="1"/>
+    <col min="14" max="14" width="6.91604566574097" customWidth="1"/>
+    <col min="15" max="15" width="8.512770652771" customWidth="1"/>
+    <col min="16" max="16" width="8.512770652771" customWidth="1"/>
+    <col min="17" max="17" width="8.512770652771" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -962,13 +962,15 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:Q1"/>
-  <pageMargins left="20" right="20" top="20" bottom="20" header="0.315" footer="0.315"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.787400" right="0.787400" top="0.787400" bottom="0.787400" header="0.315" footer="0.315"/>
+  <pageSetup paperSize="9" orientation="landscape"/>
+  <headerFooter>
+    <oddHeader>&amp;C"&amp;24&amp;U&amp;Inventory</oddHeader>
+  </headerFooter>
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c962ee68-9a8e-41da-9f50-e83b3889586b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" rightToLeft="0" displayXAxis="1" dateAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9f44759d-287f-415d-b34d-6379b512bdeb}" type="line" displayHidden="0" displayEmptyCellsAs="zero" rightToLeft="0" displayXAxis="1" dateAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="0"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>

<commit_message>
Adds Document View (Normal, Design, Print), adds footer functionality, test in progress...
</commit_message>
<xml_diff>
--- a/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample16-1.xlsx
+++ b/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample16-1.xlsx
@@ -965,12 +965,12 @@
   <pageMargins left="0.787400" right="0.787400" top="0.787400" bottom="0.787400" header="0.315" footer="0.315"/>
   <pageSetup paperSize="9" orientation="landscape"/>
   <headerFooter>
-    <oddHeader>&amp;C"&amp;24&amp;U&amp;Inventory</oddHeader>
+    <oddHeader>&amp;C&amp;24&amp;U&amp; Inventory</oddHeader>
   </headerFooter>
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9f44759d-287f-415d-b34d-6379b512bdeb}" type="line" displayHidden="0" displayEmptyCellsAs="zero" rightToLeft="0" displayXAxis="1" dateAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d6f13d5a-e0bc-49ec-8267-24954184b1d6}" type="line" displayHidden="0" displayEmptyCellsAs="zero" rightToLeft="0" displayXAxis="1" dateAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="0"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>

<commit_message>
Header and Footer sections and macros (In progress...)
</commit_message>
<xml_diff>
--- a/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample16-1.xlsx
+++ b/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample16-1.xlsx
@@ -301,7 +301,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="1" view="pageLayout"/>
+    <sheetView workbookViewId="0" showGridLines="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -965,12 +965,13 @@
   <pageMargins left="0.787400" right="0.787400" top="0.787400" bottom="0.787400" header="0.315" footer="0.315"/>
   <pageSetup paperSize="9" orientation="landscape"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;24&amp;U&amp; Inventory</oddHeader>
+    <oddHeader>&amp;L&amp;F&amp;C&amp;A&amp;RPage &amp;P / &amp;N</oddHeader>
+    <oddFooter>&amp;RPage &amp;P - &amp;N</oddFooter>
   </headerFooter>
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d6f13d5a-e0bc-49ec-8267-24954184b1d6}" type="line" displayHidden="0" displayEmptyCellsAs="zero" rightToLeft="0" displayXAxis="1" dateAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f02d4855-0372-44ad-9a42-54ab04e10481}" type="line" displayHidden="0" displayEmptyCellsAs="zero" rightToLeft="0" displayXAxis="1" dateAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="0"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>

<commit_message>
Adds FreezePanes attribute in Table model and modify XlsxWriter
</commit_message>
<xml_diff>
--- a/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample16-1.xlsx
+++ b/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample16-1.xlsx
@@ -301,14 +301,19 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="1"/>
+    <sheetView workbookViewId="0" showGridLines="1">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" state="frozen" activePane="bottomRight"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.5485782623291" customWidth="1"/>
     <col min="2" max="2" width="8.512770652771" customWidth="1"/>
     <col min="3" max="3" width="8.512770652771" customWidth="1"/>
-    <col min="4" max="4" width="8.512770652771" customWidth="1"/>
+    <col min="4" max="4" width="8.512770652771" customWidth="1" outlineLevel="1" collapsed="1" hidden="1"/>
     <col min="5" max="5" width="8.512770652771" customWidth="1"/>
     <col min="6" max="6" width="8.512770652771" customWidth="1"/>
     <col min="7" max="7" width="9.6064281463623" customWidth="1"/>
@@ -971,7 +976,7 @@
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f02d4855-0372-44ad-9a42-54ab04e10481}" type="line" displayHidden="0" displayEmptyCellsAs="zero" rightToLeft="0" displayXAxis="1" dateAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5092b519-f0ea-4521-9a82-03ee03740026}" type="line" displayHidden="0" displayEmptyCellsAs="zero" rightToLeft="0" displayXAxis="1" dateAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="0"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>

<commit_message>
Group column schema added into headers element (in progress...)
</commit_message>
<xml_diff>
--- a/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample16-1.xlsx
+++ b/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample16-1.xlsx
@@ -8,7 +8,7 @@
     <sheet name="SEKRates" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SEKRates'!$A$1:$Q$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SEKRates'!$A$2:$Q$2</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'SEKRates'!$A$1:$Q$12</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'SEKRates'!$1:$1</definedName>
   </definedNames>
@@ -17,7 +17,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Header1</t>
+  </si>
+  <si>
+    <t>Header2</t>
+  </si>
+  <si>
+    <t>Header3</t>
+  </si>
+  <si>
+    <t>Header4</t>
+  </si>
+  <si>
+    <t>Header5</t>
+  </si>
   <si>
     <t>Date</t>
   </si>
@@ -79,7 +97,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00000;[Black]\-#,##0.00000"/>
     <numFmt numFmtId="166" formatCode="##0;[Black]\-##0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -92,6 +110,12 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF" tint="0"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color rgb="FFFFFFFF" tint="0"/>
       <name val="Calibri"/>
     </font>
@@ -179,7 +203,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="16">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2">
       <alignment horizontal="left" vertical="center"/>
@@ -190,34 +214,40 @@
     <xf numFmtId="49" fontId="2" fillId="3">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="2">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="2">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="2">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="2">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="3">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="3">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="2">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="2">
+    <xf numFmtId="49" fontId="3" fillId="3">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="2">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="2">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="2">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="2">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="3">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="3">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="2">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="2">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="5" borderId="2">
@@ -227,7 +257,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0"/>
     <xf numFmtId="49" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" xfId="1">
       <alignment horizontal="left" vertical="center"/>
@@ -238,60 +268,68 @@
     <xf numFmtId="49" applyNumberFormat="1" fontId="2" applyFont="1" fillId="3" applyFill="1" xfId="3">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="4">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="5">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="6">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="7">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="8">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="9">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="3" applyBorder="1" xfId="10">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="3" applyBorder="1" xfId="11">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="2" applyBorder="1" xfId="12">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="2" applyBorder="1" xfId="13">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="2" applyFont="1" fillId="5" applyFill="1" borderId="2" applyBorder="1" xfId="14">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="2" applyFont="1" fillId="6" applyFill="1" borderId="2" applyBorder="1" xfId="15">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" xfId="4">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" xfId="5">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="6">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="7">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="8">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="9">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="10">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="11">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="3" applyBorder="1" xfId="12">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="3" applyBorder="1" xfId="13">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" applyNumberFormat="1" fontId="4" applyFont="1" fillId="4" applyFill="1" borderId="2" applyBorder="1" xfId="14">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" applyNumberFormat="1" fontId="4" applyFont="1" fillId="4" applyFill="1" borderId="2" applyBorder="1" xfId="15">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" applyNumberFormat="1" fontId="2" applyFont="1" fillId="5" applyFill="1" borderId="2" applyBorder="1" xfId="16">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" applyNumberFormat="1" fontId="2" applyFont="1" fillId="6" applyFill="1" borderId="2" applyBorder="1" xfId="17">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="16">
+  <cellStyles count="18">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="_Default_" xfId="1"/>
     <cellStyle name="HeaderStyle" xfId="2"/>
     <cellStyle name="HeaderStyle_Alternate" xfId="3"/>
-    <cellStyle name="DateValueStyle" xfId="4"/>
-    <cellStyle name="DateValueStyle_Alternate" xfId="5"/>
-    <cellStyle name="DecimalValueStyle" xfId="6"/>
-    <cellStyle name="DecimalValueStyle_Alternate" xfId="7"/>
-    <cellStyle name="SekValueStyle" xfId="8"/>
-    <cellStyle name="SekValueStyle_Alternate" xfId="9"/>
-    <cellStyle name="LastFiedlDecimalValueStyle" xfId="10"/>
-    <cellStyle name="LastFiedlDecimalValueStyle_Alternate" xfId="11"/>
-    <cellStyle name="RemarksMYRStyle" xfId="12"/>
-    <cellStyle name="RemarksMYRStyle_Alternate" xfId="13"/>
-    <cellStyle name="MaximumMYRStyle" xfId="14"/>
-    <cellStyle name="MaximumMYRStyle_Alternate" xfId="15"/>
+    <cellStyle name="HeaderTopStyle" xfId="4"/>
+    <cellStyle name="HeaderTopStyle_Alternate" xfId="5"/>
+    <cellStyle name="DateValueStyle" xfId="6"/>
+    <cellStyle name="DateValueStyle_Alternate" xfId="7"/>
+    <cellStyle name="DecimalValueStyle" xfId="8"/>
+    <cellStyle name="DecimalValueStyle_Alternate" xfId="9"/>
+    <cellStyle name="SekValueStyle" xfId="10"/>
+    <cellStyle name="SekValueStyle_Alternate" xfId="11"/>
+    <cellStyle name="LastFiedlDecimalValueStyle" xfId="12"/>
+    <cellStyle name="LastFiedlDecimalValueStyle_Alternate" xfId="13"/>
+    <cellStyle name="RemarksMYRStyle" xfId="14"/>
+    <cellStyle name="RemarksMYRStyle_Alternate" xfId="15"/>
+    <cellStyle name="MaximumMYRStyle" xfId="16"/>
+    <cellStyle name="MaximumMYRStyle_Alternate" xfId="17"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
@@ -299,674 +337,735 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="1">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" state="frozen" activePane="bottomRight"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen" activePane="bottomRight"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.5485782623291" customWidth="1"/>
-    <col min="2" max="2" width="8.512770652771" customWidth="1"/>
+    <col min="2" max="2" width="8.512770652771" customWidth="1" outlineLevel="1"/>
     <col min="3" max="3" width="8.512770652771" customWidth="1"/>
-    <col min="4" max="4" width="8.512770652771" customWidth="1" outlineLevel="1" collapsed="1" hidden="1"/>
-    <col min="5" max="5" width="8.512770652771" customWidth="1"/>
+    <col min="4" max="4" width="8.512770652771" customWidth="1"/>
+    <col min="5" max="5" width="8.512770652771" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="8.512770652771" customWidth="1"/>
     <col min="7" max="7" width="9.6064281463623" customWidth="1"/>
-    <col min="8" max="8" width="8.512770652771" customWidth="1"/>
+    <col min="8" max="8" width="8.512770652771" customWidth="1" outlineLevel="1"/>
     <col min="9" max="9" width="8.512770652771" customWidth="1"/>
     <col min="10" max="10" width="8.5311861038208" customWidth="1"/>
-    <col min="11" max="11" width="8.512770652771" customWidth="1"/>
+    <col min="11" max="11" width="8.512770652771" customWidth="1" outlineLevel="1"/>
     <col min="12" max="12" width="8.512770652771" customWidth="1"/>
     <col min="13" max="13" width="8.512770652771" customWidth="1"/>
     <col min="14" max="14" width="6.91604566574097" customWidth="1"/>
     <col min="15" max="15" width="8.512770652771" customWidth="1"/>
-    <col min="16" max="16" width="8.512770652771" customWidth="1"/>
-    <col min="17" max="17" width="8.512770652771" customWidth="1"/>
+    <col min="16" max="16" width="8.512770652771" customWidth="1" outlineLevel="2"/>
+    <col min="17" max="17" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="I1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="L1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="Q1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4">
+      <c r="L2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6">
         <v>42430</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B3" s="8">
         <v>6.1735000610351562</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C3" s="8">
         <v>6.420839786529541</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D3" s="8">
         <v>8.6478500366210937</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E3" s="8">
         <v>1.2566800117492676</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F3" s="8">
         <v>9.3737602233886719</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G3" s="8">
         <v>12.016830444335938</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H3" s="8">
         <v>1.1106699705123901</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I3" s="8">
         <v>0.075989998877048492</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J3" s="8">
         <v>2.0690000057220459</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K3" s="8">
         <v>0.99522000551223755</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L3" s="8">
         <v>5.6922698020935059</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M3" s="8">
         <v>0.11665000021457672</v>
       </c>
-      <c r="N2" s="8">
-        <v>1</v>
-      </c>
-      <c r="O2" s="6">
+      <c r="N3" s="10">
+        <v>1</v>
+      </c>
+      <c r="O3" s="8">
         <v>0.24232999980449677</v>
       </c>
-      <c r="P2" s="6">
+      <c r="P3" s="8">
         <v>2.9301700592041016</v>
       </c>
-      <c r="Q2" s="10">
+      <c r="Q3" s="12">
         <v>8.6318502426147461</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="5">
+    <row r="4">
+      <c r="A4" s="7">
         <v>42431</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B4" s="9">
         <v>6.27223014831543</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C4" s="9">
         <v>6.4234499931335449</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D4" s="9">
         <v>8.63479995727539</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E4" s="9">
         <v>1.254040002822876</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F4" s="9">
         <v>9.3535003662109375</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G4" s="9">
         <v>12.149700164794922</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H4" s="9">
         <v>1.110990047454834</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I4" s="9">
         <v>0.075819998979568481</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J4" s="16">
         <v>2.074009895324707</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K4" s="9">
         <v>0.99311000108718872</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L4" s="9">
         <v>5.7327699661254883</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M4" s="9">
         <v>0.11756999790668488</v>
       </c>
-      <c r="N3" s="9">
-        <v>1</v>
-      </c>
-      <c r="O3" s="7">
+      <c r="N4" s="11">
+        <v>1</v>
+      </c>
+      <c r="O4" s="9">
         <v>0.24305999279022217</v>
       </c>
-      <c r="P3" s="7">
+      <c r="P4" s="9">
         <v>2.9408299922943115</v>
       </c>
-      <c r="Q3" s="11">
+      <c r="Q4" s="13">
         <v>8.6381998062133789</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="4">
+    <row r="5">
+      <c r="A5" s="6">
         <v>42436</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B5" s="8">
         <v>6.3377799987792969</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C5" s="8">
         <v>6.3840298652648926</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D5" s="8">
         <v>8.5024499893188477</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E5" s="8">
         <v>1.2497999668121338</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F5" s="8">
         <v>9.32373046875</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G5" s="8">
         <v>12.057559967041016</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H5" s="8">
         <v>1.0931400060653687</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I5" s="8">
         <v>0.074780002236366272</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J5" s="8">
         <v>2.0717101097106934</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K5" s="8">
         <v>0.99751001596450806</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L5" s="8">
         <v>5.7753901481628418</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M5" s="8">
         <v>0.11841999739408493</v>
       </c>
-      <c r="N4" s="8">
-        <v>1</v>
-      </c>
-      <c r="O4" s="6">
+      <c r="N5" s="10">
+        <v>1</v>
+      </c>
+      <c r="O5" s="8">
         <v>0.23973000049591064</v>
       </c>
-      <c r="P4" s="6">
+      <c r="P5" s="8">
         <v>2.9108800888061523</v>
       </c>
-      <c r="Q4" s="10">
+      <c r="Q5" s="12">
         <v>8.4888496398925781</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="5">
+    <row r="6">
+      <c r="A6" s="7">
         <v>42437</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B6" s="9">
         <v>6.3026800155639648</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C6" s="9">
         <v>6.3177399635314941</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D6" s="9">
         <v>8.54065990447998</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E6" s="9">
         <v>1.2547099590301514</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F6" s="9">
         <v>9.3625402450561523</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G6" s="9">
         <v>12.033610343933105</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H6" s="9">
         <v>1.090459942817688</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I6" s="9">
         <v>0.075309999287128448</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J6" s="9">
         <v>2.0562500953674316</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K6" s="9">
         <v>0.99225002527236938</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L6" s="9">
         <v>5.7250099182128906</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M6" s="9">
         <v>0.11619000136852264</v>
       </c>
-      <c r="N5" s="9">
-        <v>1</v>
-      </c>
-      <c r="O5" s="7">
+      <c r="N6" s="11">
+        <v>1</v>
+      </c>
+      <c r="O6" s="9">
         <v>0.23948000371456146</v>
       </c>
-      <c r="P5" s="7">
+      <c r="P6" s="9">
         <v>2.9106700420379639</v>
       </c>
-      <c r="Q5" s="11">
+      <c r="Q6" s="13">
         <v>8.4701995849609375</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="4">
+    <row r="7">
+      <c r="A7" s="6">
         <v>42438</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B7" s="8">
         <v>6.3263001441955566</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C7" s="8">
         <v>6.336979866027832</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D7" s="8">
         <v>8.4611797332763672</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E7" s="8">
         <v>1.2439899444580078</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F7" s="8">
         <v>9.28125</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G7" s="8">
         <v>11.988789558410645</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H7" s="8">
         <v>1.0854400396347046</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I7" s="8">
         <v>0.074670001864433289</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J7" s="8">
         <v>2.0412800312042236</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K7" s="8">
         <v>0.98960000276565552</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L7" s="8">
         <v>5.7160100936889648</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M7" s="8">
         <v>0.11862999945878983</v>
       </c>
-      <c r="N6" s="8">
-        <v>1</v>
-      </c>
-      <c r="O6" s="6">
+      <c r="N7" s="10">
+        <v>1</v>
+      </c>
+      <c r="O7" s="8">
         <v>0.23893000185489655</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P7" s="8">
         <v>2.9134900569915771</v>
       </c>
-      <c r="Q6" s="10">
+      <c r="Q7" s="12">
         <v>8.4294500350952148</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="5">
+    <row r="8">
+      <c r="A8" s="7">
         <v>42439</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B8" s="9">
         <v>6.2424101829528809</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C8" s="9">
         <v>6.2881698608398437</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D8" s="9">
         <v>8.48684024810791</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E8" s="9">
         <v>1.2525999546051025</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F8" s="9">
         <v>9.3435001373291016</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G8" s="9">
         <v>11.99193000793457</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H8" s="9">
         <v>1.0795600414276123</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I8" s="9">
         <v>0.073919996619224548</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J8" s="9">
         <v>2.0450000762939453</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K8" s="9">
         <v>0.9826700091362</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L8" s="9">
         <v>5.58144998550415</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M8" s="9">
         <v>0.11768999695777893</v>
       </c>
-      <c r="N7" s="9">
-        <v>1</v>
-      </c>
-      <c r="O7" s="7">
+      <c r="N8" s="11">
+        <v>1</v>
+      </c>
+      <c r="O8" s="9">
         <v>0.2378000020980835</v>
       </c>
-      <c r="P7" s="7">
+      <c r="P8" s="9">
         <v>2.8914999961853027</v>
       </c>
-      <c r="Q7" s="11">
+      <c r="Q8" s="13">
         <v>8.3824501037597656</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="4">
+    <row r="9">
+      <c r="A9" s="6">
         <v>42440</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B9" s="8">
         <v>6.3017997741699219</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C9" s="8">
         <v>6.3015198707580566</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D9" s="8">
         <v>8.4829502105712891</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E9" s="8">
         <v>1.248479962348938</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F9" s="8">
         <v>9.3122997283935547</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G9" s="8">
         <v>12.011940002441406</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H9" s="8">
         <v>1.0754499435424805</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I9" s="8">
         <v>0.0735199972987175</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J9" s="8">
         <v>2.0411200523376465</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K9" s="8">
         <v>0.98934000730514526</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L9" s="8">
         <v>5.6233501434326172</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M9" s="8">
         <v>0.11913999915122986</v>
       </c>
-      <c r="N8" s="8">
-        <v>1</v>
-      </c>
-      <c r="O8" s="6">
+      <c r="N9" s="10">
+        <v>1</v>
+      </c>
+      <c r="O9" s="8">
         <v>0.23808999359607697</v>
       </c>
-      <c r="P8" s="6">
+      <c r="P9" s="8">
         <v>2.90310001373291</v>
       </c>
-      <c r="Q8" s="10">
+      <c r="Q9" s="12">
         <v>8.3451004028320312</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="5">
+    <row r="10">
+      <c r="A10" s="7">
         <v>42444</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B10" s="9">
         <v>6.19789981842041</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C10" s="9">
         <v>6.2161498069763184</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D10" s="9">
         <v>8.4293098449707031</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E10" s="9">
         <v>1.2375400066375732</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F10" s="9">
         <v>9.2289600372314453</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G10" s="9">
         <v>11.764180183410645</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H10" s="9">
         <v>1.0702600479125977</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I10" s="9">
         <v>0.0735900029540062</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J10" s="9">
         <v>2.0092899799346924</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K10" s="9">
         <v>0.9712899923324585</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L10" s="9">
         <v>5.4927802085876465</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M10" s="9">
         <v>0.11693999916315079</v>
       </c>
-      <c r="N9" s="9">
-        <v>1</v>
-      </c>
-      <c r="O9" s="7">
+      <c r="N10" s="11">
+        <v>1</v>
+      </c>
+      <c r="O10" s="9">
         <v>0.23642000555992126</v>
       </c>
-      <c r="P9" s="7">
+      <c r="P10" s="9">
         <v>2.8648700714111328</v>
       </c>
-      <c r="Q9" s="11">
+      <c r="Q10" s="13">
         <v>8.3053998947143555</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="4">
+    <row r="11">
+      <c r="A11" s="6">
         <v>42445</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B11" s="8">
         <v>6.1850800514221191</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C11" s="8">
         <v>6.2249298095703125</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D11" s="8">
         <v>8.4179201126098633</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E11" s="8">
         <v>1.2354300022125244</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F11" s="8">
         <v>9.2114896774292</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G11" s="8">
         <v>11.724699974060059</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H11" s="8">
         <v>1.0715199708938599</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I11" s="8">
         <v>0.073179997503757477</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J11" s="8">
         <v>2.0117900371551514</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K11" s="8">
         <v>0.96907001733779907</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L11" s="8">
         <v>5.4913802146911621</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M11" s="8">
         <v>0.1183599978685379</v>
       </c>
-      <c r="N10" s="8">
-        <v>1</v>
-      </c>
-      <c r="O10" s="6">
+      <c r="N11" s="10">
+        <v>1</v>
+      </c>
+      <c r="O11" s="8">
         <v>0.23724000155925751</v>
       </c>
-      <c r="P10" s="6">
+      <c r="P11" s="8">
         <v>2.8476700782775879</v>
       </c>
-      <c r="Q10" s="10">
+      <c r="Q11" s="12">
         <v>8.3177499771118164</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="5">
+    <row r="12">
+      <c r="A12" s="7">
         <v>42446</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B12" s="9">
         <v>6.2521400451660156</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C12" s="9">
         <v>6.306419849395752</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D12" s="9">
         <v>8.4598102569580078</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E12" s="9">
         <v>1.2432700395584106</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F12" s="9">
         <v>9.2662296295166016</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G12" s="9">
         <v>11.863960266113281</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H12" s="9">
         <v>1.0557099580764771</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I12" s="9">
         <v>0.073559999465942383</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J12" s="9">
         <v>2.0170600414276123</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K12" s="9">
         <v>0.98158997297286987</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L12" s="9">
         <v>5.5954399108886719</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M12" s="9">
         <v>0.12024000287055969</v>
       </c>
-      <c r="N11" s="9">
-        <v>1</v>
-      </c>
-      <c r="O11" s="7">
+      <c r="N12" s="11">
+        <v>1</v>
+      </c>
+      <c r="O12" s="9">
         <v>0.23543000221252441</v>
       </c>
-      <c r="P11" s="7">
+      <c r="P12" s="9">
         <v>2.8759500980377197</v>
       </c>
-      <c r="Q11" s="11">
+      <c r="Q12" s="13">
         <v>8.1882495880126953</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="4">
+    <row r="13">
+      <c r="A13" s="6">
         <v>42447</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B13" s="8">
         <v>6.2535901069641113</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C13" s="8">
         <v>6.3239998817443848</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D13" s="8">
         <v>8.4782600402832031</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E13" s="8">
         <v>1.2438100576400757</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F13" s="8">
         <v>9.2697601318359375</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G13" s="8">
         <v>11.913220405578613</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H13" s="8">
         <v>1.0588099956512451</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I13" s="8">
         <v>0.073700003325939178</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J13" s="8">
         <v>2.0255401134490967</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K13" s="8">
         <v>0.9843900203704834</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L13" s="8">
         <v>5.590670108795166</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M13" s="8">
         <v>0.12063000351190567</v>
       </c>
-      <c r="N12" s="8">
-        <v>1</v>
-      </c>
-      <c r="O12" s="6">
+      <c r="N13" s="10">
+        <v>1</v>
+      </c>
+      <c r="O13" s="8">
         <v>0.23537999391555786</v>
       </c>
-      <c r="P12" s="6">
+      <c r="P13" s="8">
         <v>2.8687999248504639</v>
       </c>
-      <c r="Q12" s="10">
+      <c r="Q13" s="12">
         <v>8.2095003128051758</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q1"/>
+  <autoFilter ref="A2:Q2"/>
+  <mergeCells>
+    <mergeCell ref="A1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+  </mergeCells>
   <pageMargins left="0.787400" right="0.787400" top="0.787400" bottom="0.787400" header="0.315" footer="0.315"/>
   <pageSetup paperSize="9" orientation="landscape"/>
   <headerFooter>
@@ -976,8 +1075,8 @@
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5092b519-f0ea-4521-9a82-03ee03740026}" type="line" displayHidden="0" displayEmptyCellsAs="zero" rightToLeft="0" displayXAxis="1" dateAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
-          <x14:colorSeries rgb="0"/>
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6a5561fb-2fa7-4d7a-bc4c-7bdfe42c5e92}" type="column" displayHidden="0" displayEmptyCellsAs="zero" rightToLeft="0" displayXAxis="1" dateAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+          <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
           <x14:colorMarkers rgb="FFD00000"/>
@@ -985,14 +1084,13 @@
           <x14:colorLast rgb="FFD00000"/>
           <x14:colorHigh rgb="FFFF0000"/>
           <x14:colorLow rgb="FFD00000"/>
-          <xm:f>'SEKRates'!A2:A12</xm:f>
+          <xm:f>'SEKRates'!A3:A13</xm:f>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'SEKRates'!B2:B12</xm:f>
+              <xm:f>'SEKRates'!B3:B13</xm:f>
               <xm:sqref>B14</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
-          <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>

</xml_diff>